<commit_message>
Eng. Requisitos: Ubuntu School (22/07/22)
</commit_message>
<xml_diff>
--- a/Engenharia de Requisitos/Template de Requisitos (Whatsapp).xlsx
+++ b/Engenharia de Requisitos/Template de Requisitos (Whatsapp).xlsx
@@ -21,7 +21,7 @@
     <author>Autor</author>
   </authors>
   <commentList>
-    <comment ref="B11" authorId="0">
+    <comment ref="B9" authorId="0">
       <text>
         <r>
           <rPr>
@@ -46,7 +46,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B12" authorId="0">
+    <comment ref="B10" authorId="0">
       <text>
         <r>
           <rPr>
@@ -60,7 +60,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B13" authorId="0">
+    <comment ref="B11" authorId="0">
       <text>
         <r>
           <rPr>
@@ -73,12 +73,36 @@
         </r>
       </text>
     </comment>
+    <comment ref="B12" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Gustavo Santos:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+quando cadastrar um contato automaticamente criar um banco de dados específico para ambos.</t>
+        </r>
+      </text>
+    </comment>
   </commentList>
 </comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="33">
   <si>
     <t>Engenharia inversa do aplicativo do whatsapp, e possíveis melhorias</t>
   </si>
@@ -159,13 +183,31 @@
   </si>
   <si>
     <t>Possibilidade de fazer o upload e download de arquivos,imagens,etc</t>
+  </si>
+  <si>
+    <t>Requisitos</t>
+  </si>
+  <si>
+    <t>Descrição do Requisito</t>
+  </si>
+  <si>
+    <t>Risco Total</t>
+  </si>
+  <si>
+    <t>Priorização</t>
+  </si>
+  <si>
+    <t>Descrição</t>
+  </si>
+  <si>
+    <t>Para o usuário sempre ter acesso as suas msg mesmo após uma ocorrência de perda ou roubo do dispositivo.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="5">
+  <fonts count="10">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -200,16 +242,70 @@
       <name val="Tahoma"/>
       <charset val="1"/>
     </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -217,22 +313,112 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -527,237 +713,478 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J24"/>
+  <dimension ref="A1:J26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I16" sqref="I16"/>
+      <selection activeCell="I26" sqref="I26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="60.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="63.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="1:10" ht="18.75">
+      <c r="A1" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="3"/>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3"/>
-      <c r="E1" s="3"/>
-      <c r="F1" s="3"/>
-      <c r="G1" s="3"/>
-      <c r="H1" s="3"/>
-      <c r="I1" s="3"/>
-      <c r="J1" s="3"/>
+      <c r="B1" s="7"/>
+      <c r="C1" s="7"/>
+      <c r="D1" s="7"/>
+      <c r="E1" s="7"/>
+      <c r="F1" s="7"/>
+      <c r="G1" s="7"/>
+      <c r="H1" s="7"/>
+      <c r="I1" s="7"/>
+      <c r="J1" s="7"/>
     </row>
     <row r="2" spans="1:10">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="4"/>
-      <c r="C2" s="4"/>
-      <c r="D2" s="4"/>
-      <c r="E2" s="4"/>
-      <c r="F2" s="4"/>
-      <c r="G2" s="4"/>
-      <c r="H2" s="4"/>
-      <c r="I2" s="4"/>
-      <c r="J2" s="4"/>
+      <c r="B2" s="8"/>
+      <c r="C2" s="8"/>
+      <c r="D2" s="8"/>
+      <c r="E2" s="8"/>
+      <c r="F2" s="8"/>
+      <c r="G2" s="8"/>
+      <c r="H2" s="8"/>
+      <c r="I2" s="8"/>
+      <c r="J2" s="8"/>
     </row>
     <row r="3" spans="1:10">
-      <c r="A3" s="4"/>
-      <c r="B3" s="4"/>
-      <c r="C3" s="4"/>
-      <c r="D3" s="4"/>
-      <c r="E3" s="4"/>
-      <c r="F3" s="4"/>
-      <c r="G3" s="4"/>
-      <c r="H3" s="4"/>
-      <c r="I3" s="4"/>
-      <c r="J3" s="4"/>
+      <c r="A3" s="8"/>
+      <c r="B3" s="8"/>
+      <c r="C3" s="8"/>
+      <c r="D3" s="8"/>
+      <c r="E3" s="8"/>
+      <c r="F3" s="8"/>
+      <c r="G3" s="8"/>
+      <c r="H3" s="8"/>
+      <c r="I3" s="8"/>
+      <c r="J3" s="8"/>
     </row>
     <row r="4" spans="1:10">
-      <c r="A4" s="4"/>
-      <c r="B4" s="4"/>
-      <c r="C4" s="4"/>
-      <c r="D4" s="4"/>
-      <c r="E4" s="4"/>
-      <c r="F4" s="4"/>
-      <c r="G4" s="4"/>
-      <c r="H4" s="4"/>
-      <c r="I4" s="4"/>
-      <c r="J4" s="4"/>
+      <c r="A4" s="8"/>
+      <c r="B4" s="8"/>
+      <c r="C4" s="8"/>
+      <c r="D4" s="8"/>
+      <c r="E4" s="8"/>
+      <c r="F4" s="8"/>
+      <c r="G4" s="8"/>
+      <c r="H4" s="8"/>
+      <c r="I4" s="8"/>
+      <c r="J4" s="8"/>
     </row>
     <row r="5" spans="1:10">
-      <c r="A5" s="4"/>
-      <c r="B5" s="4"/>
-      <c r="C5" s="4"/>
-      <c r="D5" s="4"/>
-      <c r="E5" s="4"/>
-      <c r="F5" s="4"/>
-      <c r="G5" s="4"/>
-      <c r="H5" s="4"/>
-      <c r="I5" s="4"/>
-      <c r="J5" s="4"/>
+      <c r="A5" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="C5" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="D5" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="E5" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="F5" s="12"/>
+      <c r="G5" s="12"/>
+      <c r="H5" s="12"/>
+      <c r="I5" s="12"/>
+      <c r="J5" s="12"/>
     </row>
     <row r="6" spans="1:10">
-      <c r="A6" s="4"/>
-      <c r="B6" s="4"/>
-      <c r="C6" s="4"/>
-      <c r="D6" s="4"/>
-      <c r="E6" s="4"/>
-      <c r="F6" s="4"/>
-      <c r="G6" s="4"/>
-      <c r="H6" s="4"/>
-      <c r="I6" s="4"/>
-      <c r="J6" s="4"/>
+      <c r="A6" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C6" s="10">
+        <v>10</v>
+      </c>
+      <c r="D6" s="10" t="str">
+        <f>IF(C6&lt;10,"Baixa",IF(C6&lt;15,"Médio",IF(C6&lt;20,"Alto","Elevado")))</f>
+        <v>Médio</v>
+      </c>
+      <c r="E6" s="1"/>
+      <c r="F6" s="1"/>
+      <c r="G6" s="1"/>
+      <c r="H6" s="1"/>
+      <c r="I6" s="1"/>
+      <c r="J6" s="1"/>
     </row>
     <row r="7" spans="1:10">
       <c r="A7" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>3</v>
-      </c>
+        <v>4</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C7" s="11">
+        <v>15</v>
+      </c>
+      <c r="D7" s="10" t="str">
+        <f t="shared" ref="D7:D22" si="0">IF(C7&lt;10,"Baixa",IF(C7&lt;15,"Médio",IF(C7&lt;20,"Alto","Elevado")))</f>
+        <v>Alto</v>
+      </c>
+      <c r="E7" s="1"/>
+      <c r="F7" s="1"/>
+      <c r="G7" s="1"/>
+      <c r="H7" s="1"/>
+      <c r="I7" s="1"/>
+      <c r="J7" s="1"/>
     </row>
     <row r="8" spans="1:10">
-      <c r="A8" s="2"/>
-      <c r="B8" s="1"/>
+      <c r="A8" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C8" s="11">
+        <v>8</v>
+      </c>
+      <c r="D8" s="10" t="str">
+        <f t="shared" si="0"/>
+        <v>Baixa</v>
+      </c>
+      <c r="E8" s="1"/>
+      <c r="F8" s="1"/>
+      <c r="G8" s="1"/>
+      <c r="H8" s="1"/>
+      <c r="I8" s="1"/>
+      <c r="J8" s="1"/>
     </row>
     <row r="9" spans="1:10">
       <c r="A9" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>26</v>
-      </c>
+        <v>7</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C9" s="11">
+        <v>12</v>
+      </c>
+      <c r="D9" s="10" t="str">
+        <f t="shared" si="0"/>
+        <v>Médio</v>
+      </c>
+      <c r="E9" s="1"/>
+      <c r="F9" s="1"/>
+      <c r="G9" s="1"/>
+      <c r="H9" s="1"/>
+      <c r="I9" s="1"/>
+      <c r="J9" s="1"/>
     </row>
     <row r="10" spans="1:10">
       <c r="A10" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>6</v>
-      </c>
+        <v>9</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C10" s="11">
+        <v>10</v>
+      </c>
+      <c r="D10" s="10" t="str">
+        <f t="shared" si="0"/>
+        <v>Médio</v>
+      </c>
+      <c r="E10" s="1"/>
+      <c r="F10" s="1"/>
+      <c r="G10" s="1"/>
+      <c r="H10" s="1"/>
+      <c r="I10" s="1"/>
+      <c r="J10" s="1"/>
     </row>
     <row r="11" spans="1:10">
       <c r="A11" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>8</v>
-      </c>
+        <v>11</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C11" s="11">
+        <v>15</v>
+      </c>
+      <c r="D11" s="10" t="str">
+        <f t="shared" si="0"/>
+        <v>Alto</v>
+      </c>
+      <c r="E11" s="1"/>
+      <c r="F11" s="1"/>
+      <c r="G11" s="1"/>
+      <c r="H11" s="1"/>
+      <c r="I11" s="1"/>
+      <c r="J11" s="1"/>
     </row>
     <row r="12" spans="1:10">
       <c r="A12" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>10</v>
-      </c>
+        <v>13</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C12" s="11">
+        <v>12</v>
+      </c>
+      <c r="D12" s="10" t="str">
+        <f t="shared" si="0"/>
+        <v>Médio</v>
+      </c>
+      <c r="E12" s="1"/>
+      <c r="F12" s="1"/>
+      <c r="G12" s="1"/>
+      <c r="H12" s="1"/>
+      <c r="I12" s="1"/>
+      <c r="J12" s="1"/>
     </row>
     <row r="13" spans="1:10">
       <c r="A13" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="B13" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10">
-      <c r="A14" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B14" s="1" t="s">
-        <v>14</v>
-      </c>
+      <c r="B13" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C13" s="11">
+        <v>16</v>
+      </c>
+      <c r="D13" s="10" t="str">
+        <f t="shared" si="0"/>
+        <v>Alto</v>
+      </c>
+      <c r="E13" s="1"/>
+      <c r="F13" s="1"/>
+      <c r="G13" s="1"/>
+      <c r="H13" s="1"/>
+      <c r="I13" s="1"/>
+      <c r="J13" s="1"/>
+    </row>
+    <row r="14" spans="1:10" ht="30.75" customHeight="1">
+      <c r="A14" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="B14" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="C14" s="10">
+        <v>22</v>
+      </c>
+      <c r="D14" s="10" t="str">
+        <f t="shared" si="0"/>
+        <v>Elevado</v>
+      </c>
+      <c r="E14" s="13" t="s">
+        <v>32</v>
+      </c>
+      <c r="F14" s="14"/>
+      <c r="G14" s="14"/>
+      <c r="H14" s="14"/>
+      <c r="I14" s="14"/>
+      <c r="J14" s="15"/>
     </row>
     <row r="15" spans="1:10">
       <c r="A15" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B15" s="1" t="s">
-        <v>15</v>
-      </c>
+      <c r="B15" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C15" s="11">
+        <v>8</v>
+      </c>
+      <c r="D15" s="10" t="str">
+        <f t="shared" si="0"/>
+        <v>Baixa</v>
+      </c>
+      <c r="E15" s="1"/>
+      <c r="F15" s="1"/>
+      <c r="G15" s="1"/>
+      <c r="H15" s="1"/>
+      <c r="I15" s="1"/>
+      <c r="J15" s="1"/>
     </row>
     <row r="16" spans="1:10">
       <c r="A16" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B16" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2">
+      <c r="B16" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C16" s="11">
+        <v>24</v>
+      </c>
+      <c r="D16" s="10" t="str">
+        <f t="shared" si="0"/>
+        <v>Elevado</v>
+      </c>
+      <c r="E16" s="1"/>
+      <c r="F16" s="1"/>
+      <c r="G16" s="1"/>
+      <c r="H16" s="1"/>
+      <c r="I16" s="1"/>
+      <c r="J16" s="1"/>
+    </row>
+    <row r="17" spans="1:10">
       <c r="A17" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B17" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2">
+      <c r="B17" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C17" s="11">
+        <v>16</v>
+      </c>
+      <c r="D17" s="10" t="str">
+        <f t="shared" si="0"/>
+        <v>Alto</v>
+      </c>
+      <c r="E17" s="1"/>
+      <c r="F17" s="1"/>
+      <c r="G17" s="1"/>
+      <c r="H17" s="1"/>
+      <c r="I17" s="1"/>
+      <c r="J17" s="1"/>
+    </row>
+    <row r="18" spans="1:10">
       <c r="A18" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B18" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2">
+      <c r="B18" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C18" s="11">
+        <v>10</v>
+      </c>
+      <c r="D18" s="10" t="str">
+        <f t="shared" si="0"/>
+        <v>Médio</v>
+      </c>
+      <c r="E18" s="1"/>
+      <c r="F18" s="1"/>
+      <c r="G18" s="1"/>
+      <c r="H18" s="1"/>
+      <c r="I18" s="1"/>
+      <c r="J18" s="1"/>
+    </row>
+    <row r="19" spans="1:10">
       <c r="A19" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B19" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2">
+      <c r="B19" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C19" s="11">
+        <v>8</v>
+      </c>
+      <c r="D19" s="10" t="str">
+        <f t="shared" si="0"/>
+        <v>Baixa</v>
+      </c>
+      <c r="E19" s="1"/>
+      <c r="F19" s="1"/>
+      <c r="G19" s="1"/>
+      <c r="H19" s="1"/>
+      <c r="I19" s="1"/>
+      <c r="J19" s="1"/>
+    </row>
+    <row r="20" spans="1:10">
       <c r="A20" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B20" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2">
+      <c r="B20" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C20" s="11">
+        <v>5</v>
+      </c>
+      <c r="D20" s="10" t="str">
+        <f t="shared" si="0"/>
+        <v>Baixa</v>
+      </c>
+      <c r="E20" s="1"/>
+      <c r="F20" s="1"/>
+      <c r="G20" s="1"/>
+      <c r="H20" s="1"/>
+      <c r="I20" s="1"/>
+      <c r="J20" s="1"/>
+    </row>
+    <row r="21" spans="1:10">
       <c r="A21" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="B21" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2">
+        <v>24</v>
+      </c>
+      <c r="B21" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C21" s="11">
+        <v>5</v>
+      </c>
+      <c r="D21" s="11" t="str">
+        <f t="shared" si="0"/>
+        <v>Baixa</v>
+      </c>
+      <c r="E21" s="1"/>
+      <c r="F21" s="1"/>
+      <c r="G21" s="1"/>
+      <c r="H21" s="1"/>
+      <c r="I21" s="1"/>
+      <c r="J21" s="1"/>
+    </row>
+    <row r="22" spans="1:10">
       <c r="A22" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="B22" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2">
-      <c r="A23" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="B23" s="1" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2">
-      <c r="A24" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="B24" s="1" t="s">
+      <c r="B22" s="3" t="s">
         <v>25</v>
       </c>
+      <c r="C22" s="11">
+        <v>5</v>
+      </c>
+      <c r="D22" s="11" t="str">
+        <f t="shared" si="0"/>
+        <v>Baixa</v>
+      </c>
+      <c r="E22" s="1"/>
+      <c r="F22" s="1"/>
+      <c r="G22" s="1"/>
+      <c r="H22" s="1"/>
+      <c r="I22" s="1"/>
+      <c r="J22" s="1"/>
+    </row>
+    <row r="26" spans="1:10">
+      <c r="I26" s="18"/>
     </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="20">
+    <mergeCell ref="E22:J22"/>
+    <mergeCell ref="E17:J17"/>
+    <mergeCell ref="E18:J18"/>
+    <mergeCell ref="E19:J19"/>
+    <mergeCell ref="E20:J20"/>
+    <mergeCell ref="E21:J21"/>
+    <mergeCell ref="E12:J12"/>
+    <mergeCell ref="E13:J13"/>
+    <mergeCell ref="E14:J14"/>
+    <mergeCell ref="E15:J15"/>
+    <mergeCell ref="E16:J16"/>
+    <mergeCell ref="E7:J7"/>
+    <mergeCell ref="E8:J8"/>
+    <mergeCell ref="E9:J9"/>
+    <mergeCell ref="E10:J10"/>
+    <mergeCell ref="E11:J11"/>
     <mergeCell ref="A1:J1"/>
-    <mergeCell ref="A2:J6"/>
+    <mergeCell ref="A2:J4"/>
+    <mergeCell ref="E5:J5"/>
+    <mergeCell ref="E6:J6"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="597" r:id="rId1"/>

</xml_diff>